<commit_message>
Fix removing redundant entries
When days are repeated twice we should remove first one if it is day to bay and the last one if it is a day to sell.
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -420,7 +420,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>197.060777974566</v>
+        <v>188.1070723521612</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -431,7 +431,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>174.1908819847063</v>
+        <v>156.4264313298883</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -442,7 +442,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>130.8192397157352</v>
+        <v>129.0821741183443</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -453,51 +453,51 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>121.5223522054245</v>
+        <v>120.6760754743007</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>113.7190073676539</v>
+        <v>101.7144789607758</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>106.2524485823781</v>
+        <v>94.61486169571577</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>97.09077534580342</v>
+        <v>92.23404854491551</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>88.71467273367143</v>
+        <v>88.49543971791351</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -508,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>65.45535845928678</v>
+        <v>69.90923716236374</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -519,7 +519,7 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>64.21852665799882</v>
+        <v>51.71913448807164</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -527,32 +527,32 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>44.5644819846675</v>
+        <v>44.52487332378689</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>43.45712485961867</v>
+        <v>29.43699693634931</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>26.08805737699089</v>
+        <v>20.45246752243328</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -560,32 +560,32 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>20.45246752243328</v>
+        <v>13.16876223331853</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>14.96575805808946</v>
+        <v>9.328489758797152</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>11.46816511792545</v>
+        <v>-3.223615634411131</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -593,10 +593,10 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>7.990570655975258</v>
+        <v>-7.786797665645799</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -607,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="C19">
-        <v>3.191269346815639</v>
+        <v>-16.24622036142086</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -618,7 +618,7 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>-13.39677838822663</v>
+        <v>-29.4483929612289</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -629,7 +629,7 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>-20.07866998126697</v>
+        <v>-36.99842750196777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>